<commit_message>
website & logboek update
</commit_message>
<xml_diff>
--- a/Documents/Logboeken/Logboek-Ben.xlsx
+++ b/Documents/Logboeken/Logboek-Ben.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t xml:space="preserve">Project Fifa </t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>werken aan website template.</t>
+  </si>
+  <si>
+    <t>werken aan de website</t>
   </si>
 </sst>
 </file>
@@ -498,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,6 +682,20 @@
         <v>29</v>
       </c>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>42856</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
website update 12-5-2017 &logboek
</commit_message>
<xml_diff>
--- a/Documents/Logboeken/Logboek-Ben.xlsx
+++ b/Documents/Logboeken/Logboek-Ben.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t xml:space="preserve">Project Fifa </t>
   </si>
@@ -164,6 +164,24 @@
   </si>
   <si>
     <t>werken aan de php van topscoorder.</t>
+  </si>
+  <si>
+    <t>23.30</t>
+  </si>
+  <si>
+    <t>thuis</t>
+  </si>
+  <si>
+    <t>werken aan de php van resultaten.php.</t>
+  </si>
+  <si>
+    <t>8.40</t>
+  </si>
+  <si>
+    <t>werken aan de html van invoeren teams en spelers</t>
+  </si>
+  <si>
+    <t>werken aan de php van invoeren teams en spelers</t>
   </si>
 </sst>
 </file>
@@ -537,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,6 +862,48 @@
         <v>42</v>
       </c>
     </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>42866</v>
+      </c>
+      <c r="C35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>42867</v>
+      </c>
+      <c r="C37" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>42867</v>
+      </c>
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>